<commit_message>
i make changes to some function in the formula notebook
</commit_message>
<xml_diff>
--- a/2020.xlsx
+++ b/2020.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\D\Downloads\MR AAAA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\MR AAAA\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50757EF3-D4F4-433A-A427-3BB049022559}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>9 8</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Day</t>
   </si>
@@ -56,7 +54,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -403,11 +401,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H366"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="H232" sqref="H232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,28 +415,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -6610,8 +6608,8 @@
       <c r="G231" s="1">
         <v>64</v>
       </c>
-      <c r="H231" s="1" t="s">
-        <v>0</v>
+      <c r="H231" s="1">
+        <v>98</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>